<commit_message>
limitar OIL, limiType Up 2005 maxima importacion 1000
</commit_message>
<xml_diff>
--- a/VT_REG_PRI.xlsx
+++ b/VT_REG_PRI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Caso_Base_Junio_VEDA\CasoBase_Junio_Simulacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FDC26D-401F-4BF1-95C5-23EBC90421DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5066823-00A4-430E-BD54-FCBF0DF057FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EnergyBalance" sheetId="133" r:id="rId1"/>
@@ -6091,7 +6091,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="217">
   <si>
     <t>CommName</t>
   </si>
@@ -7357,7 +7357,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7733,6 +7733,7 @@
     <xf numFmtId="0" fontId="21" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="20% - Énfasis5" xfId="1" builtinId="46"/>
@@ -12679,7 +12680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="B1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -13879,8 +13880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G49"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -14345,13 +14346,19 @@
         <f>$M$5</f>
         <v>OIL</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="E14" s="16">
+        <v>2005</v>
+      </c>
+      <c r="F14" s="211" t="s">
+        <v>206</v>
+      </c>
       <c r="G14" s="15"/>
       <c r="H14" s="134">
         <v>8</v>
       </c>
-      <c r="I14" s="132"/>
+      <c r="I14" s="132">
+        <v>1000</v>
+      </c>
       <c r="K14" s="197" t="str">
         <f>EnergyBalance!$B$6</f>
         <v>IMP</v>
@@ -15406,7 +15413,7 @@
         <v>Residential Natural Gas</v>
       </c>
       <c r="M5" s="197" t="str">
-        <f t="shared" ref="M5:M10" si="0">$E$2</f>
+        <f t="shared" ref="M5:M9" si="0">$E$2</f>
         <v>PJ</v>
       </c>
       <c r="N5" s="197"/>
@@ -15687,11 +15694,11 @@
     </row>
     <row r="17" spans="2:17">
       <c r="B17" t="str">
-        <f t="shared" ref="B17:B22" si="1">K17</f>
+        <f t="shared" ref="B17:B18" si="1">K17</f>
         <v>FTE-RSDGAS</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" ref="C17:C22" si="2">RIGHT(D17,3)</f>
+        <f t="shared" ref="C17:C18" si="2">RIGHT(D17,3)</f>
         <v>GAS</v>
       </c>
       <c r="D17" t="str">
@@ -15710,7 +15717,7 @@
       </c>
       <c r="J17" s="197"/>
       <c r="K17" s="197" t="str">
-        <f t="shared" ref="K17:K22" si="3">"FT"&amp;$G$2&amp;"-"&amp;K5</f>
+        <f t="shared" ref="K17:K18" si="3">"FT"&amp;$G$2&amp;"-"&amp;K5</f>
         <v>FTE-RSDGAS</v>
       </c>
       <c r="L17" s="200" t="str">
@@ -15718,11 +15725,11 @@
         <v>Sector Fuel Existing Residential Sector- Natural Gas</v>
       </c>
       <c r="M17" s="197" t="str">
-        <f t="shared" ref="M17:M22" si="4">$E$2</f>
+        <f t="shared" ref="M17:M21" si="4">$E$2</f>
         <v>PJ</v>
       </c>
       <c r="N17" s="197" t="str">
-        <f t="shared" ref="N17:N22" si="5">$E$2&amp;"a"</f>
+        <f t="shared" ref="N17:N21" si="5">$E$2&amp;"a"</f>
         <v>PJa</v>
       </c>
       <c r="O17" s="197"/>
@@ -16534,11 +16541,11 @@
         <v>Power Plants Existing00 - Natural Gas</v>
       </c>
       <c r="X12" s="197" t="str">
-        <f t="shared" ref="X12:X18" si="0">$E$2</f>
+        <f t="shared" ref="X12:X16" si="0">$E$2</f>
         <v>PJ</v>
       </c>
       <c r="Y12" s="197" t="str">
-        <f t="shared" ref="Y12:Y18" si="1">$F$2</f>
+        <f t="shared" ref="Y12:Y16" si="1">$F$2</f>
         <v>GW</v>
       </c>
       <c r="Z12" s="196"/>

</xml_diff>

<commit_message>
PRI GAS se quito limite MINGAS3, se adiciona limite para IMPGAS
</commit_message>
<xml_diff>
--- a/VT_REG_PRI.xlsx
+++ b/VT_REG_PRI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Caso_Base_Junio_VEDA\CasoBase_Junio_Simulacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5066823-00A4-430E-BD54-FCBF0DF057FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E08868E-13E2-4F52-8037-10FED63B91EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2352" windowWidth="17280" windowHeight="8880" tabRatio="900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EnergyBalance" sheetId="133" r:id="rId1"/>
@@ -6091,7 +6091,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="217">
   <si>
     <t>CommName</t>
   </si>
@@ -13104,8 +13104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:T34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -13517,7 +13517,7 @@
         <v>5.4</v>
       </c>
       <c r="I13" s="132">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="K13" s="197"/>
       <c r="L13" s="197"/>
@@ -13548,13 +13548,19 @@
         <f>$M$5</f>
         <v>GAS</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="E14" s="16">
+        <v>2005</v>
+      </c>
+      <c r="F14" s="211" t="s">
+        <v>206</v>
+      </c>
       <c r="G14" s="15"/>
       <c r="H14" s="134">
         <v>4.5</v>
       </c>
-      <c r="I14" s="132"/>
+      <c r="I14" s="132">
+        <v>1000</v>
+      </c>
       <c r="K14" s="197" t="str">
         <f>EnergyBalance!$B$6</f>
         <v>IMP</v>
@@ -13880,8 +13886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2"/>

</xml_diff>

<commit_message>
Se agrega cambio en Demanda
</commit_message>
<xml_diff>
--- a/VT_REG_PRI.xlsx
+++ b/VT_REG_PRI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Caso_Base_Junio_VEDA\CasoBase_Junio_Simulacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E08868E-13E2-4F52-8037-10FED63B91EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2DE2FA-FCB0-43A8-B28A-662F7908E5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2352" windowWidth="17280" windowHeight="8880" tabRatio="900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EnergyBalance" sheetId="133" r:id="rId1"/>
@@ -12680,8 +12680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="B1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -13104,7 +13104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>

</xml_diff>